<commit_message>
Add confidence interval to the statistical analysis
</commit_message>
<xml_diff>
--- a/analysis/exercise_3_statistics.xlsx
+++ b/analysis/exercise_3_statistics.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\i04.local\i2\ctx\1\RV\rv350\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEEDCCA-B875-4D91-BF4E-AB62BCDDA747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689C691E-B912-44AE-9218-AE013F353B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16050" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16050" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Low traffic densit" sheetId="1" r:id="rId1"/>
     <sheet name="Medium traffic density" sheetId="2" r:id="rId2"/>
     <sheet name="High traffic density" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="21">
   <si>
     <t>Dataset</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>Reduced Capacity</t>
+  </si>
+  <si>
+    <t>Confidence Interval</t>
   </si>
 </sst>
 </file>
@@ -494,9 +497,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z32"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="X17" sqref="X17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1530,376 +1535,390 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, C15, 10)</f>
+        <v>0.7839855938160214</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" ref="D16:L16" si="8">_xlfn.CONFIDENCE.NORM(0.05, D15, 10)</f>
+        <v>0.97013267704477424</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="8"/>
+        <v>147.94548999026145</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="8"/>
+        <v>14.074131621363335</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="8"/>
+        <v>0.38107409332032616</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="8"/>
+        <v>5.3545670266242733E-3</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="8"/>
+        <v>0.54032478230482195</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="8"/>
+        <v>0.77438893541569775</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="8"/>
+        <v>0.54032478230482195</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="8"/>
+        <v>0.18593850969136841</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="O16" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q16" s="2">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, Q15, 10)</f>
+        <v>0.62288629852494459</v>
+      </c>
+      <c r="R16" s="2">
+        <f t="shared" ref="R16" si="9">_xlfn.CONFIDENCE.NORM(0.05, R15, 10)</f>
+        <v>0.96218063573701362</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" ref="S16" si="10">_xlfn.CONFIDENCE.NORM(0.05, S15, 10)</f>
+        <v>149.71431278002848</v>
+      </c>
+      <c r="T16" s="2">
+        <f t="shared" ref="T16" si="11">_xlfn.CONFIDENCE.NORM(0.05, T15, 10)</f>
+        <v>14.090133102362088</v>
+      </c>
+      <c r="U16" s="2">
+        <f t="shared" ref="U16" si="12">_xlfn.CONFIDENCE.NORM(0.05, U15, 10)</f>
+        <v>0.3845683184872743</v>
+      </c>
+      <c r="V16" s="2" t="e">
+        <f t="shared" ref="V16" si="13">_xlfn.CONFIDENCE.NORM(0.05, V15, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W16" s="2">
+        <f t="shared" ref="W16" si="14">_xlfn.CONFIDENCE.NORM(0.05, W15, 10)</f>
+        <v>0.48407539501852548</v>
+      </c>
+      <c r="X16" s="2">
+        <f t="shared" ref="X16" si="15">_xlfn.CONFIDENCE.NORM(0.05, X15, 10)</f>
+        <v>0.91008208340456687</v>
+      </c>
+      <c r="Y16" s="2">
+        <f t="shared" ref="Y16" si="16">_xlfn.CONFIDENCE.NORM(0.05, Y15, 10)</f>
+        <v>0.48407539501852548</v>
+      </c>
+      <c r="Z16" s="2">
+        <f t="shared" ref="Z16" si="17">_xlfn.CONFIDENCE.NORM(0.05, Z15, 10)</f>
+        <v>0.18593850969136841</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>0</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C18" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M17" s="1"/>
-      <c r="O17" t="s">
+      <c r="M18" s="1"/>
+      <c r="O18" t="s">
         <v>0</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P18" t="s">
         <v>1</v>
       </c>
-      <c r="Q17" s="8" t="s">
+      <c r="Q18" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="T17" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U17" s="1" t="s">
+      <c r="U18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V17" s="1" t="s">
+      <c r="V18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="W17" s="1" t="s">
+      <c r="W18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="X17" s="1" t="s">
+      <c r="X18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Y17" s="1" t="s">
+      <c r="Y18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Z17" s="1" t="s">
+      <c r="Z18" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18">
-        <v>23</v>
-      </c>
-      <c r="D18">
-        <v>16</v>
-      </c>
-      <c r="E18" s="2">
-        <v>4740.2247690568702</v>
-      </c>
-      <c r="F18" s="2">
-        <v>579.60312499999998</v>
-      </c>
-      <c r="G18" s="2">
-        <f t="shared" ref="G18:G27" si="8">E18/F18</f>
-        <v>8.1783975354806273</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.14277442724400799</v>
-      </c>
-      <c r="I18">
-        <v>3</v>
-      </c>
-      <c r="J18" s="2">
-        <v>6.6666666670000003</v>
-      </c>
-      <c r="K18" s="3">
-        <v>4</v>
-      </c>
-      <c r="L18" s="3">
-        <v>0</v>
-      </c>
-      <c r="M18" s="3"/>
-      <c r="O18">
-        <v>1</v>
-      </c>
-      <c r="P18" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q18">
-        <v>25</v>
-      </c>
-      <c r="R18">
-        <v>17</v>
-      </c>
-      <c r="S18" s="2">
-        <v>5059.367056</v>
-      </c>
-      <c r="T18" s="2">
-        <v>578.33529399999998</v>
-      </c>
-      <c r="U18" s="2">
-        <f>S18/T18</f>
-        <v>8.748155453227449</v>
-      </c>
-      <c r="V18" s="2"/>
-      <c r="W18">
-        <v>5</v>
-      </c>
-      <c r="X18" s="2">
-        <v>11.6</v>
-      </c>
-      <c r="Y18">
-        <v>7</v>
-      </c>
-      <c r="Z18">
-        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
         <v>15</v>
       </c>
       <c r="C19">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D19">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E19" s="2">
-        <v>4488.1252733495003</v>
+        <v>4740.2247690568702</v>
       </c>
       <c r="F19" s="2">
-        <v>581.29999999999995</v>
+        <v>579.60312499999998</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="8"/>
-        <v>7.7208416881980053</v>
+        <f t="shared" ref="G19:G28" si="18">E19/F19</f>
+        <v>8.1783975354806273</v>
       </c>
       <c r="H19" s="2">
-        <v>0.175220338562454</v>
+        <v>0.14277442724400799</v>
       </c>
       <c r="I19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J19" s="2">
-        <v>21.4</v>
+        <v>6.6666666670000003</v>
       </c>
       <c r="K19" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L19" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19" s="3"/>
       <c r="O19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P19" t="s">
         <v>15</v>
       </c>
       <c r="Q19">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R19">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="S19" s="2">
-        <v>4531.0122730000003</v>
+        <v>5059.367056</v>
       </c>
       <c r="T19" s="2">
-        <v>527.19761900000003</v>
+        <v>578.33529399999998</v>
       </c>
       <c r="U19" s="2">
-        <f t="shared" ref="U19:U27" si="9">S19/T19</f>
-        <v>8.5945234001521538</v>
+        <f>S19/T19</f>
+        <v>8.748155453227449</v>
       </c>
       <c r="V19" s="2"/>
       <c r="W19">
         <v>5</v>
       </c>
       <c r="X19" s="2">
-        <v>9.6</v>
+        <v>11.6</v>
       </c>
       <c r="Y19">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="Z19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C20">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D20">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="E20" s="2">
-        <v>4959.8275708276897</v>
+        <v>4488.1252733495003</v>
       </c>
       <c r="F20" s="2">
-        <v>518.1</v>
+        <v>581.29999999999995</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="8"/>
-        <v>9.5731086099743088</v>
+        <f t="shared" si="18"/>
+        <v>7.7208416881980053</v>
       </c>
       <c r="H20" s="2">
-        <v>0.112282805343032</v>
+        <v>0.175220338562454</v>
       </c>
       <c r="I20">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J20" s="2">
-        <v>6.6666670000000003</v>
+        <v>21.4</v>
       </c>
       <c r="K20" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" s="3"/>
       <c r="O20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P20" t="s">
         <v>15</v>
       </c>
       <c r="Q20">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="R20">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="S20" s="2">
-        <v>4910.3689709999999</v>
+        <v>4531.0122730000003</v>
       </c>
       <c r="T20" s="2">
-        <v>511.1</v>
+        <v>527.19761900000003</v>
       </c>
       <c r="U20" s="2">
-        <f t="shared" si="9"/>
-        <v>9.6074524965760126</v>
+        <f t="shared" ref="U20:U28" si="19">S20/T20</f>
+        <v>8.5945234001521538</v>
       </c>
       <c r="V20" s="2"/>
       <c r="W20">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X20" s="2">
-        <v>6.6666670000000003</v>
+        <v>9.6</v>
       </c>
       <c r="Y20">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Z20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C21">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D21">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E21" s="2">
-        <v>4918.3449625418798</v>
+        <v>4959.8275708276897</v>
       </c>
       <c r="F21" s="2">
-        <v>587.00312499999995</v>
+        <v>518.1</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="8"/>
-        <v>8.3787372725517955</v>
+        <f t="shared" si="18"/>
+        <v>9.5731086099743088</v>
       </c>
       <c r="H21" s="2">
-        <v>0.14242238959450801</v>
+        <v>0.112282805343032</v>
       </c>
       <c r="I21">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J21" s="2">
-        <v>7.625</v>
+        <v>6.6666670000000003</v>
       </c>
       <c r="K21" s="3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="L21" s="3">
         <v>0</v>
       </c>
       <c r="M21" s="3"/>
       <c r="O21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P21" t="s">
         <v>15</v>
       </c>
       <c r="Q21">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="R21">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="S21" s="2">
-        <v>4678.2651759999999</v>
+        <v>4910.3689709999999</v>
       </c>
       <c r="T21" s="2">
-        <v>533.93684199999996</v>
+        <v>511.1</v>
       </c>
       <c r="U21" s="2">
-        <f t="shared" si="9"/>
-        <v>8.7618325015302094</v>
+        <f t="shared" si="19"/>
+        <v>9.6074524965760126</v>
       </c>
       <c r="V21" s="2"/>
       <c r="W21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X21" s="2">
-        <v>9.4</v>
+        <v>6.6666670000000003</v>
       </c>
       <c r="Y21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Z21">
         <v>0</v>
@@ -1907,74 +1926,74 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C22">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D22">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E22" s="2">
-        <v>4468.2778905927298</v>
+        <v>4918.3449625418798</v>
       </c>
       <c r="F22" s="2">
-        <v>588.52499999999998</v>
+        <v>587.00312499999995</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="8"/>
-        <v>7.5923331899116091</v>
+        <f t="shared" si="18"/>
+        <v>8.3787372725517955</v>
       </c>
       <c r="H22" s="2">
-        <v>0.184680142032634</v>
+        <v>0.14242238959450801</v>
       </c>
       <c r="I22">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J22" s="2">
-        <v>9.28571428571429</v>
+        <v>7.625</v>
       </c>
       <c r="K22" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M22" s="3"/>
       <c r="O22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P22" t="s">
         <v>15</v>
       </c>
       <c r="Q22">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="R22">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="S22" s="2">
-        <v>4396.5991130000002</v>
+        <v>4678.2651759999999</v>
       </c>
       <c r="T22" s="2">
-        <v>508.23333300000002</v>
+        <v>533.93684199999996</v>
       </c>
       <c r="U22" s="2">
-        <f t="shared" si="9"/>
-        <v>8.6507492278157994</v>
+        <f t="shared" si="19"/>
+        <v>8.7618325015302094</v>
       </c>
       <c r="V22" s="2"/>
       <c r="W22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="X22" s="2">
-        <v>9.8333329999999997</v>
+        <v>9.4</v>
       </c>
       <c r="Y22">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Z22">
         <v>0</v>
@@ -1982,74 +2001,74 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C23">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D23">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E23" s="2">
-        <v>5210.1881208120003</v>
+        <v>4468.2778905927298</v>
       </c>
       <c r="F23" s="2">
-        <v>604.04</v>
+        <v>588.52499999999998</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="8"/>
-        <v>8.6255680431958162</v>
+        <f t="shared" si="18"/>
+        <v>7.5923331899116091</v>
       </c>
       <c r="H23" s="2">
-        <v>0.14729599352039</v>
+        <v>0.184680142032634</v>
       </c>
       <c r="I23">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J23" s="2">
-        <v>6.25</v>
+        <v>9.28571428571429</v>
       </c>
       <c r="K23" s="3">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" s="3"/>
       <c r="O23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P23" t="s">
         <v>15</v>
       </c>
       <c r="Q23">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="R23">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="S23" s="2">
-        <v>5349.9828029999999</v>
+        <v>4396.5991130000002</v>
       </c>
       <c r="T23" s="2">
-        <v>587.50312499999995</v>
+        <v>508.23333300000002</v>
       </c>
       <c r="U23" s="2">
-        <f t="shared" si="9"/>
-        <v>9.1063052694400568</v>
+        <f t="shared" si="19"/>
+        <v>8.6507492278157994</v>
       </c>
       <c r="V23" s="2"/>
       <c r="W23">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="X23" s="2">
-        <v>6.6666670000000003</v>
+        <v>9.8333329999999997</v>
       </c>
       <c r="Y23">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Z23">
         <v>0</v>
@@ -2057,35 +2076,35 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C24">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D24">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E24" s="2">
-        <v>4286.8802706912502</v>
+        <v>5210.1881208120003</v>
       </c>
       <c r="F24" s="2">
-        <v>520.9</v>
+        <v>604.04</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="8"/>
-        <v>8.2297567108682088</v>
+        <f t="shared" si="18"/>
+        <v>8.6255680431958162</v>
       </c>
       <c r="H24" s="2">
-        <v>0.119005930378599</v>
+        <v>0.14729599352039</v>
       </c>
       <c r="I24">
         <v>4</v>
       </c>
       <c r="J24" s="2">
-        <v>10.5</v>
+        <v>6.25</v>
       </c>
       <c r="K24" s="3">
         <v>4</v>
@@ -2095,36 +2114,36 @@
       </c>
       <c r="M24" s="3"/>
       <c r="O24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P24" t="s">
         <v>15</v>
       </c>
       <c r="Q24">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R24">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="S24" s="2">
-        <v>4213.6046079999996</v>
+        <v>5349.9828029999999</v>
       </c>
       <c r="T24" s="2">
-        <v>484.647222</v>
+        <v>587.50312499999995</v>
       </c>
       <c r="U24" s="2">
-        <f t="shared" si="9"/>
-        <v>8.6941684935522012</v>
+        <f t="shared" si="19"/>
+        <v>9.1063052694400568</v>
       </c>
       <c r="V24" s="2"/>
       <c r="W24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X24" s="2">
-        <v>10.5</v>
+        <v>6.6666670000000003</v>
       </c>
       <c r="Y24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z24">
         <v>0</v>
@@ -2132,45 +2151,45 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C25">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D25">
         <v>16</v>
       </c>
       <c r="E25" s="2">
-        <v>4177.4113210181204</v>
+        <v>4286.8802706912502</v>
       </c>
       <c r="F25" s="2">
-        <v>521.00312499999995</v>
+        <v>520.9</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="8"/>
-        <v>8.0180158631833933</v>
+        <f t="shared" si="18"/>
+        <v>8.2297567108682088</v>
       </c>
       <c r="H25" s="2">
-        <v>0.13677603289948001</v>
+        <v>0.119005930378599</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J25" s="2">
-        <v>6.6666667000000004</v>
+        <v>10.5</v>
       </c>
       <c r="K25" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L25" s="3">
         <v>0</v>
       </c>
       <c r="M25" s="3"/>
       <c r="O25">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P25" t="s">
         <v>15</v>
@@ -2179,27 +2198,27 @@
         <v>21</v>
       </c>
       <c r="R25">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="S25" s="2">
-        <v>4486.7207619999999</v>
+        <v>4213.6046079999996</v>
       </c>
       <c r="T25" s="2">
-        <v>549.203125</v>
+        <v>484.647222</v>
       </c>
       <c r="U25" s="2">
-        <f t="shared" si="9"/>
-        <v>8.1695106195908842</v>
+        <f t="shared" si="19"/>
+        <v>8.6941684935522012</v>
       </c>
       <c r="V25" s="2"/>
       <c r="W25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="X25" s="2">
-        <v>6.6666670000000003</v>
+        <v>10.5</v>
       </c>
       <c r="Y25">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Z25">
         <v>0</v>
@@ -2207,45 +2226,45 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C26">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D26">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E26" s="2">
-        <v>4781.322695328</v>
+        <v>4177.4113210181204</v>
       </c>
       <c r="F26" s="2">
-        <v>565.54333333299996</v>
+        <v>521.00312499999995</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="8"/>
-        <v>8.4543878665309791</v>
+        <f t="shared" si="18"/>
+        <v>8.0180158631833933</v>
       </c>
       <c r="H26" s="2">
-        <v>0.12541146099898601</v>
+        <v>0.13677603289948001</v>
       </c>
       <c r="I26">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J26" s="2">
-        <v>6</v>
+        <v>6.6666667000000004</v>
       </c>
       <c r="K26" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L26" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M26" s="3"/>
       <c r="O26">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P26" t="s">
         <v>15</v>
@@ -2254,17 +2273,17 @@
         <v>21</v>
       </c>
       <c r="R26">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="S26" s="2">
-        <v>5101.7167579999996</v>
+        <v>4486.7207619999999</v>
       </c>
       <c r="T26" s="2">
-        <v>525.77857100000006</v>
+        <v>549.203125</v>
       </c>
       <c r="U26" s="2">
-        <f t="shared" si="9"/>
-        <v>9.7031660082624391</v>
+        <f t="shared" si="19"/>
+        <v>8.1695106195908842</v>
       </c>
       <c r="V26" s="2"/>
       <c r="W26">
@@ -2274,7 +2293,7 @@
         <v>6.6666670000000003</v>
       </c>
       <c r="Y26">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Z26">
         <v>0</v>
@@ -2282,264 +2301,428 @@
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C27">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D27">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E27" s="2">
-        <v>4963.2944316755002</v>
+        <v>4781.322695328</v>
       </c>
       <c r="F27" s="2">
-        <v>618.16999999999996</v>
+        <v>565.54333333299996</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" si="8"/>
-        <v>8.0290121352953072</v>
+        <f t="shared" si="18"/>
+        <v>8.4543878665309791</v>
       </c>
       <c r="H27" s="2">
-        <v>0.179872048872355</v>
+        <v>0.12541146099898601</v>
       </c>
       <c r="I27">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J27" s="2">
-        <v>10.875</v>
+        <v>6</v>
       </c>
       <c r="K27" s="3">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M27" s="3"/>
       <c r="O27">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P27" t="s">
         <v>15</v>
       </c>
       <c r="Q27">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="R27">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="S27" s="2">
-        <v>4896.2133560000002</v>
+        <v>5101.7167579999996</v>
       </c>
       <c r="T27" s="2">
-        <v>581.83000000000004</v>
+        <v>525.77857100000006</v>
       </c>
       <c r="U27" s="2">
-        <f t="shared" si="9"/>
-        <v>8.4151957719608816</v>
+        <f t="shared" si="19"/>
+        <v>9.7031660082624391</v>
       </c>
       <c r="V27" s="2"/>
       <c r="W27">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X27" s="2">
-        <v>14.166667</v>
+        <v>6.6666670000000003</v>
       </c>
       <c r="Y27">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Z27">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <v>20</v>
+      </c>
+      <c r="E28" s="2">
+        <v>4963.2944316755002</v>
+      </c>
+      <c r="F28" s="2">
+        <v>618.16999999999996</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="18"/>
+        <v>8.0290121352953072</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.179872048872355</v>
+      </c>
+      <c r="I28">
+        <v>8</v>
+      </c>
+      <c r="J28" s="2">
+        <v>10.875</v>
+      </c>
+      <c r="K28" s="3">
+        <v>9</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0</v>
+      </c>
+      <c r="M28" s="3"/>
+      <c r="O28">
+        <v>10</v>
+      </c>
+      <c r="P28" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q28">
+        <v>25</v>
+      </c>
+      <c r="R28">
+        <v>20</v>
+      </c>
+      <c r="S28" s="2">
+        <v>4896.2133560000002</v>
+      </c>
+      <c r="T28" s="2">
+        <v>581.83000000000004</v>
+      </c>
+      <c r="U28" s="2">
+        <f t="shared" si="19"/>
+        <v>8.4151957719608816</v>
+      </c>
+      <c r="V28" s="2"/>
+      <c r="W28">
+        <v>6</v>
+      </c>
+      <c r="X28" s="2">
+        <v>14.166667</v>
+      </c>
+      <c r="Y28">
+        <v>6</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7">
-        <f t="shared" ref="C28:L28" si="10">AVERAGE(C18:C27)</f>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7">
+        <f t="shared" ref="C29:L29" si="20">AVERAGE(C19:C28)</f>
         <v>23.4</v>
       </c>
-      <c r="D28" s="7">
-        <f t="shared" si="10"/>
+      <c r="D29" s="7">
+        <f t="shared" si="20"/>
         <v>16.899999999999999</v>
       </c>
-      <c r="E28" s="7">
-        <f t="shared" si="10"/>
+      <c r="E29" s="7">
+        <f t="shared" si="20"/>
         <v>4699.3897305893543</v>
       </c>
-      <c r="F28" s="7">
-        <f t="shared" si="10"/>
+      <c r="F29" s="7">
+        <f t="shared" si="20"/>
         <v>568.41877083329996</v>
       </c>
-      <c r="G28" s="7">
-        <f t="shared" si="10"/>
+      <c r="G29" s="7">
+        <f t="shared" si="20"/>
         <v>8.280015891519005</v>
       </c>
-      <c r="H28" s="7">
-        <f t="shared" si="10"/>
+      <c r="H29" s="7">
+        <f t="shared" si="20"/>
         <v>0.14657415694464462</v>
       </c>
-      <c r="I28" s="7">
-        <f t="shared" si="10"/>
+      <c r="I29" s="7">
+        <f t="shared" si="20"/>
         <v>5</v>
       </c>
-      <c r="J28" s="7">
-        <f t="shared" si="10"/>
+      <c r="J29" s="7">
+        <f t="shared" si="20"/>
         <v>9.1935714652714289</v>
       </c>
-      <c r="K28" s="7">
-        <f t="shared" si="10"/>
+      <c r="K29" s="7">
+        <f t="shared" si="20"/>
         <v>5.3</v>
       </c>
-      <c r="L28" s="7">
-        <f t="shared" si="10"/>
+      <c r="L29" s="7">
+        <f t="shared" si="20"/>
         <v>0.3</v>
       </c>
-      <c r="M28" s="7"/>
-      <c r="O28" s="6" t="s">
+      <c r="M29" s="7"/>
+      <c r="O29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="7">
-        <f>AVERAGE(Q18:Q27)</f>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="7">
+        <f>AVERAGE(Q19:Q28)</f>
         <v>23.3</v>
       </c>
-      <c r="R28" s="7">
-        <f>AVERAGE(R18:R27)</f>
+      <c r="R29" s="7">
+        <f>AVERAGE(R19:R28)</f>
         <v>17.7</v>
       </c>
-      <c r="S28" s="7">
-        <f>AVERAGE(S18:S27)</f>
+      <c r="S29" s="7">
+        <f>AVERAGE(S19:S28)</f>
         <v>4762.3850875999997</v>
       </c>
-      <c r="T28" s="7">
-        <f>AVERAGE(T18:T27)</f>
+      <c r="T29" s="7">
+        <f>AVERAGE(T19:T28)</f>
         <v>538.77651309999987</v>
       </c>
-      <c r="U28" s="7">
-        <f t="shared" ref="U28:V28" si="11">AVERAGE(U18:U27)</f>
+      <c r="U29" s="7">
+        <f t="shared" ref="U29:V29" si="21">AVERAGE(U19:U28)</f>
         <v>8.8451059242108094</v>
       </c>
-      <c r="V28" s="7" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W28" s="7">
-        <f>AVERAGE(W18:W27)</f>
+      <c r="V29" s="7" t="e">
+        <f t="shared" si="21"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W29" s="7">
+        <f>AVERAGE(W19:W28)</f>
         <v>4.3</v>
       </c>
-      <c r="X28" s="7">
-        <f>AVERAGE(X18:X27)</f>
+      <c r="X29" s="7">
+        <f>AVERAGE(X19:X28)</f>
         <v>9.1766668000000013</v>
       </c>
-      <c r="Y28" s="7">
-        <f>AVERAGE(Y18:Y27)</f>
+      <c r="Y29" s="7">
+        <f>AVERAGE(Y19:Y28)</f>
         <v>4.5999999999999996</v>
       </c>
-      <c r="Z28" s="7">
-        <f>AVERAGE(Z18:Z27)</f>
+      <c r="Z29" s="7">
+        <f>AVERAGE(Z19:Z28)</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="2">
-        <f t="shared" ref="C29:L29" si="12">_xlfn.STDEV.P(C18:C27)</f>
+      <c r="C30" s="2">
+        <f t="shared" ref="C30:L30" si="22">_xlfn.STDEV.P(C19:C28)</f>
         <v>2.5768197453450252</v>
       </c>
-      <c r="D29" s="2">
-        <f t="shared" si="12"/>
+      <c r="D30" s="2">
+        <f t="shared" si="22"/>
         <v>2.6627053911388696</v>
       </c>
-      <c r="E29" s="2">
-        <f t="shared" si="12"/>
+      <c r="E30" s="2">
+        <f t="shared" si="22"/>
         <v>315.49664468227411</v>
       </c>
-      <c r="F29" s="2">
-        <f t="shared" si="12"/>
+      <c r="F30" s="2">
+        <f t="shared" si="22"/>
         <v>34.396562583056742</v>
       </c>
-      <c r="G29" s="2">
-        <f t="shared" si="12"/>
+      <c r="G30" s="2">
+        <f t="shared" si="22"/>
         <v>0.52552155317863214</v>
       </c>
-      <c r="H29" s="2">
-        <f t="shared" si="12"/>
+      <c r="H30" s="2">
+        <f t="shared" si="22"/>
         <v>2.4276289746912972E-2</v>
       </c>
-      <c r="I29" s="2">
-        <f t="shared" si="12"/>
+      <c r="I30" s="2">
+        <f t="shared" si="22"/>
         <v>1.8973665961010275</v>
       </c>
-      <c r="J29" s="2">
-        <f t="shared" si="12"/>
+      <c r="J30" s="2">
+        <f t="shared" si="22"/>
         <v>4.4047589622140988</v>
       </c>
-      <c r="K29" s="2">
-        <f t="shared" si="12"/>
+      <c r="K30" s="2">
+        <f t="shared" si="22"/>
         <v>2.0024984394500787</v>
       </c>
-      <c r="L29" s="2">
-        <f t="shared" si="12"/>
+      <c r="L30" s="2">
+        <f t="shared" si="22"/>
         <v>0.45825756949558399</v>
       </c>
-      <c r="M29" s="2"/>
-      <c r="O29" t="s">
+      <c r="M30" s="2"/>
+      <c r="O30" t="s">
         <v>14</v>
       </c>
-      <c r="Q29" s="2">
-        <f>_xlfn.STDEV.P(Q18:Q27)</f>
+      <c r="Q30" s="2">
+        <f>_xlfn.STDEV.P(Q19:Q28)</f>
         <v>2.5317977802344327</v>
       </c>
-      <c r="R29" s="2">
-        <f>_xlfn.STDEV.P(R18:R27)</f>
+      <c r="R30" s="2">
+        <f>_xlfn.STDEV.P(R19:R28)</f>
         <v>2.3685438564654024</v>
       </c>
-      <c r="S29" s="2">
-        <f>_xlfn.STDEV.P(S18:S27)</f>
+      <c r="S30" s="2">
+        <f>_xlfn.STDEV.P(S19:S28)</f>
         <v>340.58542770936015</v>
       </c>
-      <c r="T29" s="2">
-        <f>_xlfn.STDEV.P(T18:T27)</f>
+      <c r="T30" s="2">
+        <f>_xlfn.STDEV.P(T19:T28)</f>
         <v>32.949646295921454</v>
       </c>
-      <c r="U29" s="2">
-        <f t="shared" ref="U29:V29" si="13">_xlfn.STDEV.P(U18:U27)</f>
+      <c r="U30" s="2">
+        <f t="shared" ref="U30:V30" si="23">_xlfn.STDEV.P(U19:U28)</f>
         <v>0.46546732950226966</v>
       </c>
-      <c r="V29" s="2" t="e">
-        <f t="shared" si="13"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W29" s="2">
-        <f>_xlfn.STDEV.P(W18:W27)</f>
+      <c r="V30" s="2" t="e">
+        <f t="shared" si="23"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W30" s="2">
+        <f>_xlfn.STDEV.P(W19:W28)</f>
         <v>1.1874342087037917</v>
       </c>
-      <c r="X29" s="2">
-        <f>_xlfn.STDEV.P(X18:X27)</f>
+      <c r="X30" s="2">
+        <f>_xlfn.STDEV.P(X19:X28)</f>
         <v>2.416289547035114</v>
       </c>
-      <c r="Y29" s="2">
-        <f>_xlfn.STDEV.P(Y18:Y27)</f>
+      <c r="Y30" s="2">
+        <f>_xlfn.STDEV.P(Y19:Y28)</f>
         <v>1.3564659966250536</v>
       </c>
-      <c r="Z29" s="2">
-        <f>_xlfn.STDEV.P(Z18:Z27)</f>
+      <c r="Z30" s="2">
+        <f>_xlfn.STDEV.P(Z19:Z28)</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="H30" s="2"/>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="2">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, C30, 10)</f>
+        <v>1.5971000773091515</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" ref="D31" si="24">_xlfn.CONFIDENCE.NORM(0.05, D30, 10)</f>
+        <v>1.6503315739184456</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" ref="E31" si="25">_xlfn.CONFIDENCE.NORM(0.05, E30, 10)</f>
+        <v>195.5432530828308</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" ref="F31" si="26">_xlfn.CONFIDENCE.NORM(0.05, F30, 10)</f>
+        <v>21.318818617331523</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" ref="G31" si="27">_xlfn.CONFIDENCE.NORM(0.05, G30, 10)</f>
+        <v>0.32571564802909359</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" ref="H31" si="28">_xlfn.CONFIDENCE.NORM(0.05, H30, 10)</f>
+        <v>1.5046323787922818E-2</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" ref="I31" si="29">_xlfn.CONFIDENCE.NORM(0.05, I30, 10)</f>
+        <v>1.1759783907240322</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" ref="J31" si="30">_xlfn.CONFIDENCE.NORM(0.05, J30, 10)</f>
+        <v>2.7300477232792937</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" ref="K31" si="31">_xlfn.CONFIDENCE.NORM(0.05, K30, 10)</f>
+        <v>1.2411385849687953</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" ref="L31" si="32">_xlfn.CONFIDENCE.NORM(0.05, L30, 10)</f>
+        <v>0.28402576508932531</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="O31" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q31" s="2">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, Q30, 10)</f>
+        <v>1.5691956869890169</v>
+      </c>
+      <c r="R31" s="2">
+        <f t="shared" ref="R31" si="33">_xlfn.CONFIDENCE.NORM(0.05, R30, 10)</f>
+        <v>1.4680117160327446</v>
+      </c>
+      <c r="S31" s="2">
+        <f t="shared" ref="S31" si="34">_xlfn.CONFIDENCE.NORM(0.05, S30, 10)</f>
+        <v>211.09315616958571</v>
+      </c>
+      <c r="T31" s="2">
+        <f t="shared" ref="T31" si="35">_xlfn.CONFIDENCE.NORM(0.05, T30, 10)</f>
+        <v>20.422027090404509</v>
+      </c>
+      <c r="U31" s="2">
+        <f t="shared" ref="U31" si="36">_xlfn.CONFIDENCE.NORM(0.05, U30, 10)</f>
+        <v>0.28849433852557715</v>
+      </c>
+      <c r="V31" s="2" t="e">
+        <f t="shared" ref="V31" si="37">_xlfn.CONFIDENCE.NORM(0.05, V30, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W31" s="2">
+        <f t="shared" ref="W31" si="38">_xlfn.CONFIDENCE.NORM(0.05, W30, 10)</f>
+        <v>0.73596582374310782</v>
+      </c>
+      <c r="X31" s="2">
+        <f t="shared" ref="X31" si="39">_xlfn.CONFIDENCE.NORM(0.05, X30, 10)</f>
+        <v>1.4976042578618025</v>
+      </c>
+      <c r="Y31" s="2">
+        <f t="shared" ref="Y31" si="40">_xlfn.CONFIDENCE.NORM(0.05, Y30, 10)</f>
+        <v>0.84073088619826419</v>
+      </c>
+      <c r="Z31" s="2">
+        <f t="shared" ref="Z31" si="41">_xlfn.CONFIDENCE.NORM(0.05, Z30, 10)</f>
+        <v>0.18593850969136841</v>
+      </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="H32" t="s">
+      <c r="H32" s="2"/>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2556,9 +2739,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z32"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Z17" sqref="Z17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3571,489 +3756,503 @@
         <v>3.0016662039607267</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, C15, 10)</f>
+        <v>2.6880818517533358</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" ref="D16:L16" si="6">_xlfn.CONFIDENCE.NORM(0.05, D15, 10)</f>
+        <v>1.2717130822289378</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="6"/>
+        <v>50.656554632876407</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="6"/>
+        <v>5.6650179958264122</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="6"/>
+        <v>0.16309297842237117</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="6"/>
+        <v>2.9873701396447284E-2</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="6"/>
+        <v>3.361209661961214</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="6"/>
+        <v>3.1179697026746558</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="6"/>
+        <v>1.9804366831405389</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="6"/>
+        <v>1.9293453804989416</v>
+      </c>
+      <c r="O16" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q16" s="2">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, Q15, 10)</f>
+        <v>2.444853763520439</v>
+      </c>
+      <c r="R16" s="2">
+        <f t="shared" ref="R16:Z16" si="7">_xlfn.CONFIDENCE.NORM(0.05, R15, 10)</f>
+        <v>1.6860247706702445</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" si="7"/>
+        <v>50.17464830816219</v>
+      </c>
+      <c r="T16" s="2">
+        <f t="shared" si="7"/>
+        <v>6.1239020167002449</v>
+      </c>
+      <c r="U16" s="2">
+        <f t="shared" si="7"/>
+        <v>0.20011409070547526</v>
+      </c>
+      <c r="V16" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W16" s="2">
+        <f t="shared" si="7"/>
+        <v>3.5653032462438388</v>
+      </c>
+      <c r="X16" s="2">
+        <f t="shared" si="7"/>
+        <v>3.1096183786324061</v>
+      </c>
+      <c r="Y16" s="2">
+        <f t="shared" si="7"/>
+        <v>1.6584584756987413</v>
+      </c>
+      <c r="Z16" s="2">
+        <f t="shared" si="7"/>
+        <v>1.8604178018513489</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>0</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>1</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O17" t="s">
+      <c r="O18" t="s">
         <v>0</v>
       </c>
-      <c r="P17" t="s">
+      <c r="P18" t="s">
         <v>1</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="Q18" t="s">
         <v>2</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="S17" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="T17" s="1" t="s">
+      <c r="T18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U17" s="1" t="s">
+      <c r="U18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="V17" s="1" t="s">
+      <c r="V18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="W17" s="1" t="s">
+      <c r="W18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="X17" s="1" t="s">
+      <c r="X18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Y17" s="1" t="s">
+      <c r="Y18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="Z17" s="1" t="s">
+      <c r="Z18" s="1" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18">
-        <v>158</v>
-      </c>
-      <c r="D18">
-        <v>101</v>
-      </c>
-      <c r="E18" s="2">
-        <v>4169.6757416205901</v>
-      </c>
-      <c r="F18" s="2">
-        <v>546.12821782178196</v>
-      </c>
-      <c r="G18" s="2">
-        <f t="shared" ref="G18:G27" si="6">E18/F18</f>
-        <v>7.6349758271990273</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.91120313498790995</v>
-      </c>
-      <c r="I18">
-        <v>59</v>
-      </c>
-      <c r="J18" s="2">
-        <v>7.1016949152542397</v>
-      </c>
-      <c r="K18">
-        <v>67</v>
-      </c>
-      <c r="L18">
-        <v>19</v>
-      </c>
-      <c r="O18">
-        <v>1</v>
-      </c>
-      <c r="P18" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q18">
-        <v>169</v>
-      </c>
-      <c r="R18">
-        <v>101</v>
-      </c>
-      <c r="S18" s="2">
-        <v>4241.0420869999998</v>
-      </c>
-      <c r="T18" s="2">
-        <v>519.56831699999998</v>
-      </c>
-      <c r="U18" s="2">
-        <f>S18/T18</f>
-        <v>8.1626264501420707</v>
-      </c>
-      <c r="W18">
-        <v>35</v>
-      </c>
-      <c r="X18" s="2">
-        <v>6.2</v>
-      </c>
-      <c r="Y18">
-        <v>36</v>
-      </c>
-      <c r="Z18">
-        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="9">
-        <v>148</v>
+      <c r="C19">
+        <v>158</v>
       </c>
       <c r="D19">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="E19" s="2">
-        <v>3666.1062516249399</v>
+        <v>4169.6757416205901</v>
       </c>
       <c r="F19" s="2">
-        <v>500.32352941176498</v>
+        <v>546.12821782178196</v>
       </c>
       <c r="G19" s="2">
-        <f t="shared" si="6"/>
-        <v>7.3274711983568217</v>
+        <f t="shared" ref="G19:G28" si="8">E19/F19</f>
+        <v>7.6349758271990273</v>
       </c>
       <c r="H19" s="2">
-        <v>0.75650790993554895</v>
+        <v>0.91120313498790995</v>
       </c>
       <c r="I19">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="J19" s="2">
-        <v>7.5833332999999996</v>
+        <v>7.1016949152542397</v>
       </c>
       <c r="K19">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="L19">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="O19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P19" t="s">
         <v>15</v>
       </c>
       <c r="Q19">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="R19">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="S19" s="2">
-        <v>4113.2071459999997</v>
+        <v>4241.0420869999998</v>
       </c>
       <c r="T19" s="2">
-        <v>498.83532600000001</v>
+        <v>519.56831699999998</v>
       </c>
       <c r="U19" s="2">
-        <f t="shared" ref="U19:U27" si="7">S19/T19</f>
-        <v>8.2456212132819147</v>
-      </c>
-      <c r="V19" s="2"/>
+        <f>S19/T19</f>
+        <v>8.1626264501420707</v>
+      </c>
       <c r="W19">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="X19" s="2">
-        <v>17.935483999999999</v>
+        <v>6.2</v>
       </c>
       <c r="Y19">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Z19">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="9">
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="D20">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E20" s="2">
-        <v>3715.1805563173498</v>
+        <v>3666.1062516249399</v>
       </c>
       <c r="F20" s="2">
-        <v>496.375</v>
+        <v>500.32352941176498</v>
       </c>
       <c r="G20" s="2">
-        <f t="shared" si="6"/>
-        <v>7.4846246412840083</v>
+        <f t="shared" si="8"/>
+        <v>7.3274711983568217</v>
       </c>
       <c r="H20" s="2">
-        <v>0.87801800158121901</v>
+        <v>0.75650790993554895</v>
       </c>
       <c r="I20">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="J20" s="2">
-        <v>8</v>
+        <v>7.5833332999999996</v>
       </c>
       <c r="K20">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="L20">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="O20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P20" t="s">
         <v>15</v>
       </c>
       <c r="Q20">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="R20">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="S20" s="2">
-        <v>3962.9801819999998</v>
+        <v>4113.2071459999997</v>
       </c>
       <c r="T20" s="2">
-        <v>488.13620700000001</v>
+        <v>498.83532600000001</v>
       </c>
       <c r="U20" s="2">
-        <f t="shared" si="7"/>
-        <v>8.1185950256707748</v>
+        <f t="shared" ref="U20:U28" si="9">S20/T20</f>
+        <v>8.2456212132819147</v>
       </c>
       <c r="V20" s="2"/>
       <c r="W20">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="X20" s="2">
-        <v>6.7575760000000002</v>
+        <v>17.935483999999999</v>
       </c>
       <c r="Y20">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Z20">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="9">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="D21">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E21" s="2">
-        <v>3753.1046722368801</v>
+        <v>3715.1805563173498</v>
       </c>
       <c r="F21" s="2">
-        <v>504.91354166669998</v>
+        <v>496.375</v>
       </c>
       <c r="G21" s="2">
-        <f t="shared" si="6"/>
-        <v>7.4331630319282533</v>
+        <f t="shared" si="8"/>
+        <v>7.4846246412840083</v>
       </c>
       <c r="H21" s="2">
-        <v>0.79966317231164896</v>
+        <v>0.87801800158121901</v>
       </c>
       <c r="I21">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="J21" s="2">
-        <v>6.3333332999999996</v>
+        <v>8</v>
       </c>
       <c r="K21">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="L21">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="O21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P21" t="s">
         <v>15</v>
       </c>
       <c r="Q21">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="R21">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="S21" s="2">
-        <v>3804.573175</v>
+        <v>3962.9801819999998</v>
       </c>
       <c r="T21" s="2">
-        <v>474.213776</v>
+        <v>488.13620700000001</v>
       </c>
       <c r="U21" s="2">
-        <f t="shared" si="7"/>
-        <v>8.0229073206004884</v>
+        <f t="shared" si="9"/>
+        <v>8.1185950256707748</v>
       </c>
       <c r="V21" s="2"/>
       <c r="W21">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="X21" s="2">
-        <v>16.629629999999999</v>
+        <v>6.7575760000000002</v>
       </c>
       <c r="Y21">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="Z21">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C22" s="9">
-        <v>181</v>
+        <v>148</v>
       </c>
       <c r="D22">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E22" s="2">
-        <v>3695.9154167349002</v>
+        <v>3753.1046722368801</v>
       </c>
       <c r="F22" s="2">
-        <v>481.52040816326502</v>
+        <v>504.91354166669998</v>
       </c>
       <c r="G22" s="2">
-        <f t="shared" si="6"/>
-        <v>7.6755114717417285</v>
+        <f t="shared" si="8"/>
+        <v>7.4331630319282533</v>
       </c>
       <c r="H22" s="2">
-        <v>0.84160326539679098</v>
+        <v>0.79966317231164896</v>
       </c>
       <c r="I22">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="J22" s="2">
-        <v>7.83673469387755</v>
+        <v>6.3333332999999996</v>
       </c>
       <c r="K22">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="L22">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P22" t="s">
         <v>15</v>
       </c>
       <c r="Q22">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="R22">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="S22" s="2">
-        <v>3891.2866680000002</v>
+        <v>3804.573175</v>
       </c>
       <c r="T22" s="2">
-        <v>462.51406300000002</v>
+        <v>474.213776</v>
       </c>
       <c r="U22" s="2">
-        <f t="shared" si="7"/>
-        <v>8.4133369756586198</v>
+        <f t="shared" si="9"/>
+        <v>8.0229073206004884</v>
       </c>
       <c r="V22" s="2"/>
       <c r="W22">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="X22" s="2">
-        <v>7.4583329999999997</v>
+        <v>16.629629999999999</v>
       </c>
       <c r="Y22">
         <v>24</v>
       </c>
       <c r="Z22">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C23" s="9">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D23">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="E23" s="2">
-        <v>3861.4096512134502</v>
+        <v>3695.9154167349002</v>
       </c>
       <c r="F23" s="2">
-        <v>534.59367816092004</v>
+        <v>481.52040816326502</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" si="6"/>
-        <v>7.2230739138129367</v>
+        <f t="shared" si="8"/>
+        <v>7.6755114717417285</v>
       </c>
       <c r="H23" s="2">
-        <v>0.81070380785793195</v>
+        <v>0.84160326539679098</v>
       </c>
       <c r="I23">
+        <v>49</v>
+      </c>
+      <c r="J23" s="2">
+        <v>7.83673469387755</v>
+      </c>
+      <c r="K23">
         <v>62</v>
       </c>
-      <c r="J23" s="2">
-        <v>6.1935483870967696</v>
-      </c>
-      <c r="K23">
-        <v>70</v>
-      </c>
       <c r="L23">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="O23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="P23" t="s">
         <v>15</v>
@@ -4062,220 +4261,220 @@
         <v>161</v>
       </c>
       <c r="R23">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="S23" s="2">
-        <v>4012.2084559999998</v>
+        <v>3891.2866680000002</v>
       </c>
       <c r="T23" s="2">
-        <v>487.672527</v>
+        <v>462.51406300000002</v>
       </c>
       <c r="U23" s="2">
-        <f t="shared" si="7"/>
-        <v>8.2272595519821028</v>
+        <f t="shared" si="9"/>
+        <v>8.4133369756586198</v>
       </c>
       <c r="V23" s="2"/>
       <c r="W23">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="X23" s="2">
-        <v>8.8108109999999993</v>
+        <v>7.4583329999999997</v>
       </c>
       <c r="Y23">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="Z23">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="9">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="D24">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="E24" s="2">
-        <v>3765.5085450500001</v>
+        <v>3861.4096512134502</v>
       </c>
       <c r="F24" s="2">
-        <v>532.55841584158395</v>
+        <v>534.59367816092004</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="6"/>
-        <v>7.0706018965064983</v>
+        <f t="shared" si="8"/>
+        <v>7.2230739138129367</v>
       </c>
       <c r="H24" s="2">
-        <v>0.87573879999048099</v>
+        <v>0.81070380785793195</v>
       </c>
       <c r="I24">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="J24" s="2">
-        <v>5.8085106382978697</v>
+        <v>6.1935483870967696</v>
       </c>
       <c r="K24">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="L24">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="O24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="P24" t="s">
         <v>15</v>
       </c>
       <c r="Q24">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="R24">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="S24" s="2">
-        <v>3769.7358009999998</v>
+        <v>4012.2084559999998</v>
       </c>
       <c r="T24" s="2">
-        <v>479.96785699999998</v>
+        <v>487.672527</v>
       </c>
       <c r="U24" s="2">
-        <f t="shared" si="7"/>
-        <v>7.8541422014432936</v>
+        <f t="shared" si="9"/>
+        <v>8.2272595519821028</v>
       </c>
       <c r="V24" s="2"/>
       <c r="W24">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="X24" s="2">
-        <v>14.56</v>
+        <v>8.8108109999999993</v>
       </c>
       <c r="Y24">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="Z24">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C25" s="9">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="D25">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E25" s="2">
-        <v>4002.6993699562099</v>
+        <v>3765.5085450500001</v>
       </c>
       <c r="F25" s="2">
-        <v>550.66105263157897</v>
+        <v>532.55841584158395</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="6"/>
-        <v>7.2688986279809136</v>
+        <f t="shared" si="8"/>
+        <v>7.0706018965064983</v>
       </c>
       <c r="H25" s="2">
-        <v>0.88673982697217202</v>
+        <v>0.87573879999048099</v>
       </c>
       <c r="I25">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="J25" s="2">
-        <v>5.59649122807018</v>
+        <v>5.8085106382978697</v>
       </c>
       <c r="K25">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="L25">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="O25">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="P25" t="s">
         <v>15</v>
       </c>
       <c r="Q25">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="R25">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="S25" s="2">
-        <v>4228.2773850000003</v>
+        <v>3769.7358009999998</v>
       </c>
       <c r="T25" s="2">
-        <v>520.54510900000002</v>
+        <v>479.96785699999998</v>
       </c>
       <c r="U25" s="2">
-        <f t="shared" si="7"/>
-        <v>8.1227876545085351</v>
+        <f t="shared" si="9"/>
+        <v>7.8541422014432936</v>
       </c>
       <c r="V25" s="2"/>
       <c r="W25">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="X25" s="2">
-        <v>4.6666670000000003</v>
+        <v>14.56</v>
       </c>
       <c r="Y25">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Z25">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C26" s="9">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="D26">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E26" s="2">
-        <v>3797.5452887718102</v>
+        <v>4002.6993699562099</v>
       </c>
       <c r="F26" s="2">
-        <v>532.24190476190495</v>
+        <v>550.66105263157897</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="6"/>
-        <v>7.1349986816062856</v>
+        <f t="shared" si="8"/>
+        <v>7.2688986279809136</v>
       </c>
       <c r="H26" s="2">
-        <v>0.98544205208833802</v>
+        <v>0.88673982697217202</v>
       </c>
       <c r="I26">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J26" s="2">
-        <v>5.5344827586206904</v>
+        <v>5.59649122807018</v>
       </c>
       <c r="K26">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="L26">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="O26">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P26" t="s">
         <v>15</v>
@@ -4284,290 +4483,452 @@
         <v>173</v>
       </c>
       <c r="R26">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="S26" s="2">
-        <v>3926.334742</v>
+        <v>4228.2773850000003</v>
       </c>
       <c r="T26" s="2">
-        <v>498.66616199999999</v>
+        <v>520.54510900000002</v>
       </c>
       <c r="U26" s="2">
-        <f t="shared" si="7"/>
-        <v>7.8736738948812013</v>
+        <f t="shared" si="9"/>
+        <v>8.1227876545085351</v>
       </c>
       <c r="V26" s="2"/>
       <c r="W26">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="X26" s="2">
-        <v>7.5</v>
+        <v>4.6666670000000003</v>
       </c>
       <c r="Y26">
         <v>25</v>
       </c>
       <c r="Z26">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C27" s="9">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D27">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E27" s="2">
-        <v>3626.4529817215798</v>
+        <v>3797.5452887718102</v>
       </c>
       <c r="F27" s="2">
-        <v>487.112871287129</v>
+        <v>532.24190476190495</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" si="6"/>
-        <v>7.4447898946689195</v>
+        <f t="shared" si="8"/>
+        <v>7.1349986816062856</v>
       </c>
       <c r="H27" s="2">
-        <v>0.85595036482068398</v>
+        <v>0.98544205208833802</v>
       </c>
       <c r="I27">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="J27" s="2">
-        <v>5</v>
+        <v>5.5344827586206904</v>
       </c>
       <c r="K27">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="L27">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="O27">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P27" t="s">
         <v>15</v>
       </c>
       <c r="Q27">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="R27">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="S27" s="2">
-        <v>3812.5956890000002</v>
+        <v>3926.334742</v>
       </c>
       <c r="T27" s="2">
-        <v>470.437273</v>
+        <v>498.66616199999999</v>
       </c>
       <c r="U27" s="2">
-        <f t="shared" si="7"/>
-        <v>8.1043656780996614</v>
-      </c>
+        <f t="shared" si="9"/>
+        <v>7.8736738948812013</v>
+      </c>
+      <c r="V27" s="2"/>
       <c r="W27">
         <v>28</v>
       </c>
       <c r="X27" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="Y27">
+        <v>25</v>
+      </c>
+      <c r="Z27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="9">
+        <v>172</v>
+      </c>
+      <c r="D28">
+        <v>101</v>
+      </c>
+      <c r="E28" s="2">
+        <v>3626.4529817215798</v>
+      </c>
+      <c r="F28" s="2">
+        <v>487.112871287129</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="8"/>
+        <v>7.4447898946689195</v>
+      </c>
+      <c r="H28" s="2">
+        <v>0.85595036482068398</v>
+      </c>
+      <c r="I28">
+        <v>51</v>
+      </c>
+      <c r="J28" s="2">
+        <v>5</v>
+      </c>
+      <c r="K28">
+        <v>48</v>
+      </c>
+      <c r="L28">
+        <v>21</v>
+      </c>
+      <c r="O28">
+        <v>10</v>
+      </c>
+      <c r="P28" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q28">
+        <v>169</v>
+      </c>
+      <c r="R28">
+        <v>110</v>
+      </c>
+      <c r="S28" s="2">
+        <v>3812.5956890000002</v>
+      </c>
+      <c r="T28" s="2">
+        <v>470.437273</v>
+      </c>
+      <c r="U28" s="2">
+        <f t="shared" si="9"/>
+        <v>8.1043656780996614</v>
+      </c>
+      <c r="W28">
+        <v>28</v>
+      </c>
+      <c r="X28" s="2">
         <v>6.4285709999999998</v>
       </c>
-      <c r="Y27">
+      <c r="Y28">
         <v>33</v>
       </c>
-      <c r="Z27">
+      <c r="Z28">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="7">
-        <f t="shared" ref="C28:L28" si="8">AVERAGE(C18:C27)</f>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7">
+        <f t="shared" ref="C29:L29" si="10">AVERAGE(C19:C28)</f>
         <v>165.1</v>
       </c>
-      <c r="D28" s="7">
-        <f t="shared" si="8"/>
+      <c r="D29" s="7">
+        <f t="shared" si="10"/>
         <v>96.7</v>
       </c>
-      <c r="E28" s="7">
-        <f t="shared" si="8"/>
+      <c r="E29" s="7">
+        <f t="shared" si="10"/>
         <v>3805.3598475247718</v>
       </c>
-      <c r="F28" s="7">
-        <f t="shared" si="8"/>
+      <c r="F29" s="7">
+        <f t="shared" si="10"/>
         <v>516.64286197466288</v>
       </c>
-      <c r="G28" s="7">
-        <f t="shared" si="8"/>
+      <c r="G29" s="7">
+        <f t="shared" si="10"/>
         <v>7.3698109185085388</v>
       </c>
-      <c r="H28" s="7">
-        <f t="shared" si="8"/>
+      <c r="H29" s="7">
+        <f t="shared" si="10"/>
         <v>0.86015703359427254</v>
       </c>
-      <c r="I28" s="7">
-        <f t="shared" si="8"/>
+      <c r="I29" s="7">
+        <f t="shared" si="10"/>
         <v>52.7</v>
       </c>
-      <c r="J28" s="7">
-        <f t="shared" si="8"/>
+      <c r="J29" s="7">
+        <f t="shared" si="10"/>
         <v>6.4988129221217292</v>
       </c>
-      <c r="K28" s="7">
-        <f t="shared" si="8"/>
+      <c r="K29" s="7">
+        <f t="shared" si="10"/>
         <v>60.3</v>
       </c>
-      <c r="L28" s="7">
-        <f t="shared" si="8"/>
+      <c r="L29" s="7">
+        <f t="shared" si="10"/>
         <v>20.7</v>
       </c>
-      <c r="O28" s="6" t="s">
+      <c r="O29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P28" s="6"/>
-      <c r="Q28" s="7">
-        <f t="shared" ref="Q28:Z28" si="9">AVERAGE(Q18:Q27)</f>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="7">
+        <f t="shared" ref="Q29:Z29" si="11">AVERAGE(Q19:Q28)</f>
         <v>165.3</v>
       </c>
-      <c r="R28" s="7">
-        <f t="shared" si="9"/>
+      <c r="R29" s="7">
+        <f t="shared" si="11"/>
         <v>96.4</v>
       </c>
-      <c r="S28" s="7">
-        <f t="shared" si="9"/>
+      <c r="S29" s="7">
+        <f t="shared" si="11"/>
         <v>3976.2241330999996</v>
       </c>
-      <c r="T28" s="7">
-        <f t="shared" si="9"/>
+      <c r="T29" s="7">
+        <f t="shared" si="11"/>
         <v>490.05566170000003</v>
       </c>
-      <c r="U28" s="7">
-        <f t="shared" si="9"/>
+      <c r="U29" s="7">
+        <f t="shared" si="11"/>
         <v>8.1145315966268665</v>
       </c>
-      <c r="V28" s="7" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W28" s="7">
-        <f t="shared" si="9"/>
+      <c r="V29" s="7" t="e">
+        <f t="shared" si="11"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W29" s="7">
+        <f t="shared" si="11"/>
         <v>29.8</v>
       </c>
-      <c r="X28" s="7">
-        <f t="shared" si="9"/>
+      <c r="X29" s="7">
+        <f t="shared" si="11"/>
         <v>9.6947071999999999</v>
       </c>
-      <c r="Y28" s="7">
-        <f t="shared" si="9"/>
+      <c r="Y29" s="7">
+        <f t="shared" si="11"/>
         <v>30</v>
       </c>
-      <c r="Z28" s="7">
-        <f t="shared" si="9"/>
+      <c r="Z29" s="7">
+        <f t="shared" si="11"/>
         <v>10.6</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>14</v>
       </c>
-      <c r="C29" s="2">
-        <f t="shared" ref="C29:L29" si="10">_xlfn.STDEV.P(C18:C27)</f>
+      <c r="C30" s="2">
+        <f t="shared" ref="C30:L30" si="12">_xlfn.STDEV.P(C19:C28)</f>
         <v>11.802118453904791</v>
       </c>
-      <c r="D29" s="2">
-        <f t="shared" si="10"/>
+      <c r="D30" s="2">
+        <f t="shared" si="12"/>
         <v>6.0174745533321525</v>
       </c>
-      <c r="E29" s="2">
-        <f t="shared" si="10"/>
+      <c r="E30" s="2">
+        <f t="shared" si="12"/>
         <v>158.33507314420186</v>
       </c>
-      <c r="F29" s="2">
-        <f t="shared" si="10"/>
+      <c r="F30" s="2">
+        <f t="shared" si="12"/>
         <v>24.012041163700033</v>
       </c>
-      <c r="G29" s="2">
-        <f t="shared" si="10"/>
+      <c r="G30" s="2">
+        <f t="shared" si="12"/>
         <v>0.19098515685828341</v>
       </c>
-      <c r="H29" s="2">
-        <f t="shared" si="10"/>
+      <c r="H30" s="2">
+        <f t="shared" si="12"/>
         <v>6.0647092965867185E-2</v>
       </c>
-      <c r="I29" s="2">
-        <f t="shared" si="10"/>
+      <c r="I30" s="2">
+        <f t="shared" si="12"/>
         <v>8.9</v>
       </c>
-      <c r="J29" s="2">
-        <f t="shared" si="10"/>
+      <c r="J30" s="2">
+        <f t="shared" si="12"/>
         <v>1.0085084492383163</v>
       </c>
-      <c r="K29" s="2">
-        <f t="shared" si="10"/>
+      <c r="K30" s="2">
+        <f t="shared" si="12"/>
         <v>10.169070754006976</v>
       </c>
-      <c r="L29" s="2">
-        <f t="shared" si="10"/>
+      <c r="L30" s="2">
+        <f t="shared" si="12"/>
         <v>3.6891733491393435</v>
       </c>
-      <c r="O29" t="s">
+      <c r="O30" t="s">
         <v>14</v>
       </c>
-      <c r="Q29" s="2">
-        <f t="shared" ref="Q29:Z29" si="11">_xlfn.STDEV.P(Q18:Q27)</f>
+      <c r="Q30" s="2">
+        <f t="shared" ref="Q30:Z30" si="13">_xlfn.STDEV.P(Q19:Q28)</f>
         <v>7.1421285342676386</v>
       </c>
-      <c r="R29" s="2">
-        <f t="shared" si="11"/>
+      <c r="R30" s="2">
+        <f t="shared" si="13"/>
         <v>6.1188234163113417</v>
       </c>
-      <c r="S29" s="2">
-        <f t="shared" si="11"/>
+      <c r="S30" s="2">
+        <f t="shared" si="13"/>
         <v>162.01021103937762</v>
       </c>
-      <c r="T29" s="2">
-        <f t="shared" si="11"/>
+      <c r="T30" s="2">
+        <f t="shared" si="13"/>
         <v>18.593923894192216</v>
       </c>
-      <c r="U29" s="2">
-        <f t="shared" si="11"/>
+      <c r="U30" s="2">
+        <f t="shared" si="13"/>
         <v>0.1599649794188619</v>
       </c>
-      <c r="V29" s="2" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W29" s="2">
-        <f t="shared" si="11"/>
+      <c r="V30" s="2" t="e">
+        <f t="shared" si="13"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W30" s="2">
+        <f t="shared" si="13"/>
         <v>4.0199502484483558</v>
       </c>
-      <c r="X29" s="2">
-        <f t="shared" si="11"/>
+      <c r="X30" s="2">
+        <f t="shared" si="13"/>
         <v>4.5504127759704787</v>
       </c>
-      <c r="Y29" s="2">
-        <f t="shared" si="11"/>
+      <c r="Y30" s="2">
+        <f t="shared" si="13"/>
         <v>5.0990195135927845</v>
       </c>
-      <c r="Z29" s="2">
-        <f t="shared" si="11"/>
+      <c r="Z30" s="2">
+        <f t="shared" si="13"/>
         <v>3.0066592756745814</v>
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="H31" t="s">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="2">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, C30, 10)</f>
+        <v>7.3148943884001802</v>
+      </c>
+      <c r="D31" s="2">
+        <f t="shared" ref="D31:L31" si="14">_xlfn.CONFIDENCE.NORM(0.05, D30, 10)</f>
+        <v>3.7296008351743772</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="14"/>
+        <v>98.135291774355679</v>
+      </c>
+      <c r="F31" s="2">
+        <f t="shared" si="14"/>
+        <v>14.882543828753921</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="14"/>
+        <v>0.11837165146467149</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="14"/>
+        <v>3.7588766943957394E-2</v>
+      </c>
+      <c r="I31" s="2">
+        <f t="shared" si="14"/>
+        <v>5.5161757875105968</v>
+      </c>
+      <c r="J31" s="2">
+        <f t="shared" si="14"/>
+        <v>0.6250685268750853</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="14"/>
+        <v>6.3027395364871239</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" si="14"/>
+        <v>2.2865313151069464</v>
+      </c>
+      <c r="O31" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q31" s="2">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, Q30, 10)</f>
+        <v>4.426655785619741</v>
+      </c>
+      <c r="R31" s="2">
+        <f t="shared" ref="R31:Z31" si="15">_xlfn.CONFIDENCE.NORM(0.05, R30, 10)</f>
+        <v>3.7924163569785949</v>
+      </c>
+      <c r="S31" s="2">
+        <f t="shared" si="15"/>
+        <v>100.41312398481986</v>
+      </c>
+      <c r="T31" s="2">
+        <f t="shared" si="15"/>
+        <v>11.52442166066942</v>
+      </c>
+      <c r="U31" s="2">
+        <f t="shared" si="15"/>
+        <v>9.9145499586512018E-2</v>
+      </c>
+      <c r="V31" s="2" t="e">
+        <f t="shared" si="15"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W31" s="2">
+        <f t="shared" si="15"/>
+        <v>2.4915451940997784</v>
+      </c>
+      <c r="X31" s="2">
+        <f t="shared" si="15"/>
+        <v>2.8203232334817119</v>
+      </c>
+      <c r="Y31" s="2">
+        <f t="shared" si="15"/>
+        <v>3.1603469641488289</v>
+      </c>
+      <c r="Z31" s="2">
+        <f t="shared" si="15"/>
+        <v>1.8635124828955363</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>17</v>
       </c>
     </row>
@@ -4584,9 +4945,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4598,14 +4959,28 @@
     <col min="8" max="8" width="19.140625" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" customWidth="1"/>
     <col min="10" max="10" width="21.42578125" customWidth="1"/>
+    <col min="15" max="16" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" customWidth="1"/>
+    <col min="18" max="18" width="16" customWidth="1"/>
+    <col min="19" max="19" width="20.28515625" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" customWidth="1"/>
+    <col min="21" max="21" width="15" customWidth="1"/>
+    <col min="22" max="22" width="15.5703125" customWidth="1"/>
+    <col min="23" max="23" width="13.85546875" customWidth="1"/>
+    <col min="24" max="24" width="21.140625" customWidth="1"/>
+    <col min="25" max="25" width="12.42578125" customWidth="1"/>
+    <col min="26" max="26" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C1" s="12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="Q1" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -4642,8 +5017,44 @@
       <c r="L3" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O3" t="s">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4681,8 +5092,25 @@
       <c r="L4" s="3">
         <v>604</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>12</v>
+      </c>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2" t="e">
+        <f t="shared" ref="U4:U13" si="1">S4/T4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V4" s="2"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4720,8 +5148,25 @@
       <c r="L5" s="3">
         <v>628</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V5" s="2"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -4759,8 +5204,25 @@
       <c r="L6" s="3">
         <v>610</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6" t="s">
+        <v>12</v>
+      </c>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V6" s="2"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -4798,8 +5260,25 @@
       <c r="L7" s="3">
         <v>572</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O7">
+        <v>4</v>
+      </c>
+      <c r="P7" t="s">
+        <v>12</v>
+      </c>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V7" s="2"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -4837,8 +5316,25 @@
       <c r="L8" s="3">
         <v>587</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O8">
+        <v>5</v>
+      </c>
+      <c r="P8" t="s">
+        <v>12</v>
+      </c>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V8" s="2"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="2"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -4876,8 +5372,25 @@
       <c r="L9" s="3">
         <v>617</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O9">
+        <v>6</v>
+      </c>
+      <c r="P9" t="s">
+        <v>12</v>
+      </c>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V9" s="2"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -4915,8 +5428,25 @@
       <c r="L10" s="3">
         <v>574</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O10">
+        <v>7</v>
+      </c>
+      <c r="P10" t="s">
+        <v>12</v>
+      </c>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V10" s="2"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="2"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -4954,8 +5484,25 @@
       <c r="L11" s="3">
         <v>618</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O11">
+        <v>8</v>
+      </c>
+      <c r="P11" t="s">
+        <v>12</v>
+      </c>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V11" s="2"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -4993,8 +5540,25 @@
       <c r="L12" s="3">
         <v>589</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O12">
+        <v>9</v>
+      </c>
+      <c r="P12" t="s">
+        <v>12</v>
+      </c>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V12" s="2"/>
+      <c r="W12" s="3"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="3"/>
+      <c r="Z12" s="3"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -5032,172 +5596,397 @@
       <c r="L13" s="3">
         <v>608</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O13">
+        <v>10</v>
+      </c>
+      <c r="P13" t="s">
+        <v>12</v>
+      </c>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V13" s="2"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="5"/>
+      <c r="Y13" s="3"/>
+      <c r="Z13" s="3"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="7">
-        <f t="shared" ref="C14" si="1">AVERAGE(C4:C13)</f>
+        <f t="shared" ref="C14" si="2">AVERAGE(C4:C13)</f>
         <v>2409.9</v>
       </c>
       <c r="D14" s="7">
-        <f t="shared" ref="D14:L14" si="2">AVERAGE(D4:D13)</f>
+        <f t="shared" ref="D14:L14" si="3">AVERAGE(D4:D13)</f>
         <v>1810.3</v>
       </c>
       <c r="E14" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3771.4300483691941</v>
       </c>
       <c r="F14" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>295.35081954325534</v>
       </c>
       <c r="G14" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12.769625405249766</v>
       </c>
       <c r="H14" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10.639400789626769</v>
       </c>
       <c r="I14" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5052.1000000000004</v>
       </c>
       <c r="J14" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.4157302549581221</v>
       </c>
       <c r="K14" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2993.9</v>
       </c>
       <c r="L14" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>600.70000000000005</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="7" t="e">
+        <f t="shared" ref="Q14:Z14" si="4">AVERAGE(Q4:Q13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R14" s="7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S14" s="7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T14" s="7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U14" s="7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V14" s="7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W14" s="7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X14" s="7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y14" s="7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Z14" s="7" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="C15" s="2">
-        <f t="shared" ref="C15" si="3">_xlfn.STDEV.P(C4:C13)</f>
+        <f t="shared" ref="C15" si="5">_xlfn.STDEV.P(C4:C13)</f>
         <v>8.2030482139263334</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" ref="D15:L15" si="4">_xlfn.STDEV.P(D4:D13)</f>
+        <f t="shared" ref="D15:L15" si="6">_xlfn.STDEV.P(D4:D13)</f>
         <v>11.925183436744275</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>38.019631480797941</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>2.7333882058938102</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.10136644274312469</v>
       </c>
       <c r="H15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.20236135989615284</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>137.40629534340849</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.28181822654560257</v>
       </c>
       <c r="K15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>87.499085709508989</v>
       </c>
       <c r="L15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>18.226628870967886</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="O15" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q15" s="2" t="e">
+        <f t="shared" ref="Q15:Z15" si="7">_xlfn.STDEV.P(Q4:Q13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R15" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S15" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T15" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U15" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V15" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W15" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X15" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y15" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Z15" s="2" t="e">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, C15, 10)</f>
+        <v>5.084208532746346</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" ref="D16:L16" si="8">_xlfn.CONFIDENCE.NORM(0.05, D15, 10)</f>
+        <v>7.3911694534147383</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="8"/>
+        <v>23.56437872184868</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="8"/>
+        <v>1.6941404313728612</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="8"/>
+        <v>6.2826417654573447E-2</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="8"/>
+        <v>0.125422565594031</v>
+      </c>
+      <c r="I16" s="2">
+        <f t="shared" si="8"/>
+        <v>85.16373926121797</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" si="8"/>
+        <v>0.17466953682584596</v>
+      </c>
+      <c r="K16" s="2">
+        <f t="shared" si="8"/>
+        <v>54.231498653944712</v>
+      </c>
+      <c r="L16" s="2">
+        <f t="shared" si="8"/>
+        <v>11.296774029884791</v>
+      </c>
+      <c r="O16" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q16" s="2" t="e">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, Q15, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R16" s="2" t="e">
+        <f t="shared" ref="R16" si="9">_xlfn.CONFIDENCE.NORM(0.05, R15, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S16" s="2" t="e">
+        <f t="shared" ref="S16" si="10">_xlfn.CONFIDENCE.NORM(0.05, S15, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T16" s="2" t="e">
+        <f t="shared" ref="T16" si="11">_xlfn.CONFIDENCE.NORM(0.05, T15, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U16" s="2" t="e">
+        <f t="shared" ref="U16" si="12">_xlfn.CONFIDENCE.NORM(0.05, U15, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V16" s="2" t="e">
+        <f t="shared" ref="V16" si="13">_xlfn.CONFIDENCE.NORM(0.05, V15, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W16" s="2" t="e">
+        <f t="shared" ref="W16" si="14">_xlfn.CONFIDENCE.NORM(0.05, W15, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X16" s="2" t="e">
+        <f t="shared" ref="X16" si="15">_xlfn.CONFIDENCE.NORM(0.05, X15, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y16" s="2" t="e">
+        <f t="shared" ref="Y16" si="16">_xlfn.CONFIDENCE.NORM(0.05, Y15, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Z16" s="2" t="e">
+        <f t="shared" ref="Z16" si="17">_xlfn.CONFIDENCE.NORM(0.05, Z15, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>0</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C18" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L18" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="O18" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" t="s">
+      <c r="Q18" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" t="e">
-        <f t="shared" ref="G18:G27" si="5">E18/F18</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H18" s="2"/>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="9"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="G19:G28" si="18">E19/F19</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H19" s="2"/>
       <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>15</v>
+      </c>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" t="e">
+        <f t="shared" ref="U19:U28" si="19">S19/T19</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V19" s="2"/>
+      <c r="X19" s="2"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>15</v>
@@ -5206,15 +5995,30 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H20" s="2"/>
       <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O20">
+        <v>2</v>
+      </c>
+      <c r="P20" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q20" s="9"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V20" s="2"/>
+      <c r="X20" s="2"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>15</v>
@@ -5223,15 +6027,30 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H21" s="2"/>
       <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O21">
+        <v>3</v>
+      </c>
+      <c r="P21" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q21" s="9"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V21" s="2"/>
+      <c r="X21" s="2"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>15</v>
@@ -5240,15 +6059,30 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H22" s="2"/>
       <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O22">
+        <v>4</v>
+      </c>
+      <c r="P22" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q22" s="9"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V22" s="2"/>
+      <c r="X22" s="2"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="9" t="s">
         <v>15</v>
@@ -5257,15 +6091,30 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H23" s="2"/>
       <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O23">
+        <v>5</v>
+      </c>
+      <c r="P23" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="9"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V23" s="2"/>
+      <c r="X23" s="2"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>15</v>
@@ -5274,15 +6123,30 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H24" s="2"/>
       <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O24">
+        <v>6</v>
+      </c>
+      <c r="P24" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q24" s="9"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V24" s="2"/>
+      <c r="X24" s="2"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>15</v>
@@ -5291,15 +6155,30 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H25" s="2"/>
       <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O25">
+        <v>7</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q25" s="9"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V25" s="2"/>
+      <c r="X25" s="2"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" s="9" t="s">
         <v>15</v>
@@ -5308,15 +6187,30 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H26" s="2"/>
       <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O26">
+        <v>8</v>
+      </c>
+      <c r="P26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q26" s="9"/>
+      <c r="S26" s="2"/>
+      <c r="T26" s="2"/>
+      <c r="U26" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V26" s="2"/>
+      <c r="X26" s="2"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" s="9" t="s">
         <v>15</v>
@@ -5325,101 +6219,313 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" t="e">
-        <f t="shared" si="5"/>
+        <f t="shared" si="18"/>
         <v>#DIV/0!</v>
       </c>
       <c r="H27" s="2"/>
       <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+      <c r="O27">
+        <v>9</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q27" s="9"/>
+      <c r="S27" s="2"/>
+      <c r="T27" s="2"/>
+      <c r="U27" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V27" s="2"/>
+      <c r="X27" s="2"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" t="e">
+        <f t="shared" si="18"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="O28">
+        <v>10</v>
+      </c>
+      <c r="P28" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q28" s="9"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" t="e">
+        <f t="shared" si="19"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V28" s="2"/>
+      <c r="X28" s="2"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="7" t="e">
-        <f>AVERAGE(D18:D27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E28" s="7" t="e">
-        <f>AVERAGE(E18:E27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F28" s="7" t="e">
-        <f>AVERAGE(F18:F27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G28" s="7" t="e">
-        <f>AVERAGE(G18:G27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="7" t="e">
-        <f>AVERAGE(I18:I27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J28" s="7" t="e">
-        <f>AVERAGE(J18:J27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K28" s="7" t="e">
-        <f>AVERAGE(K18:K27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L28" s="7" t="e">
-        <f>AVERAGE(L18:L27)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="7" t="e">
+        <f>AVERAGE(D19:D28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E29" s="7" t="e">
+        <f>AVERAGE(E19:E28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F29" s="7" t="e">
+        <f>AVERAGE(F19:F28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G29" s="7" t="e">
+        <f>AVERAGE(G19:G28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H29" s="7" t="e">
+        <f>AVERAGE(H19:H28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I29" s="7" t="e">
+        <f>AVERAGE(I19:I28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J29" s="7" t="e">
+        <f>AVERAGE(J19:J28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K29" s="7" t="e">
+        <f>AVERAGE(K19:K28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L29" s="7" t="e">
+        <f>AVERAGE(L19:L28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O29" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="7" t="e">
+        <f>AVERAGE(R19:R28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S29" s="7" t="e">
+        <f>AVERAGE(S19:S28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T29" s="7" t="e">
+        <f>AVERAGE(T19:T28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U29" s="7" t="e">
+        <f>AVERAGE(U19:U28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V29" s="7" t="e">
+        <f>AVERAGE(V19:V28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W29" s="7" t="e">
+        <f>AVERAGE(W19:W28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X29" s="7" t="e">
+        <f>AVERAGE(X19:X28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y29" s="7" t="e">
+        <f>AVERAGE(Y19:Y28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Z29" s="7" t="e">
+        <f>AVERAGE(Z19:Z28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>14</v>
       </c>
-      <c r="D29" t="e">
-        <f>_xlfn.STDEV.P(D18:D27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E29" t="e">
-        <f>_xlfn.STDEV.P(E18:E27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F29" t="e">
-        <f>_xlfn.STDEV.P(F18:F27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G29" t="e">
-        <f>_xlfn.STDEV.P(G18:G27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H29" s="7" t="e">
-        <f>AVERAGE(H18:H27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I29" t="e">
-        <f>_xlfn.STDEV.P(I18:I27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J29" t="e">
-        <f>_xlfn.STDEV.P(J18:J27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K29" t="e">
-        <f>_xlfn.STDEV.P(K18:K27)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L29" t="e">
-        <f>_xlfn.STDEV.P(L18:L27)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D30" t="e">
+        <f>_xlfn.STDEV.P(D19:D28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E30" t="e">
+        <f>_xlfn.STDEV.P(E19:E28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F30" t="e">
+        <f>_xlfn.STDEV.P(F19:F28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G30" t="e">
+        <f>_xlfn.STDEV.P(G19:G28)</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="H30" s="2" t="e">
-        <f>_xlfn.STDEV.P(H18:H27)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H32" t="s">
+        <f>_xlfn.STDEV.P(H19:H28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I30" t="e">
+        <f>_xlfn.STDEV.P(I19:I28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J30" t="e">
+        <f>_xlfn.STDEV.P(J19:J28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K30" t="e">
+        <f>_xlfn.STDEV.P(K19:K28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L30" t="e">
+        <f>_xlfn.STDEV.P(L19:L28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O30" t="s">
+        <v>14</v>
+      </c>
+      <c r="R30" t="e">
+        <f>_xlfn.STDEV.P(R19:R28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S30" t="e">
+        <f>_xlfn.STDEV.P(S19:S28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T30" t="e">
+        <f>_xlfn.STDEV.P(T19:T28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U30" t="e">
+        <f>_xlfn.STDEV.P(U19:U28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V30" s="2" t="e">
+        <f>_xlfn.STDEV.P(V19:V28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W30" t="e">
+        <f>_xlfn.STDEV.P(W19:W28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X30" t="e">
+        <f>_xlfn.STDEV.P(X19:X28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y30" t="e">
+        <f>_xlfn.STDEV.P(Y19:Y28)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Z30" t="e">
+        <f>_xlfn.STDEV.P(Z19:Z28)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="2" t="e">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, C30, 10)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="D31" s="2" t="e">
+        <f t="shared" ref="D31:L31" si="20">_xlfn.CONFIDENCE.NORM(0.05, D30, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E31" s="2" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F31" s="2" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G31" s="2" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H31" s="2" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" s="2" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J31" s="2" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K31" s="2" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L31" s="2" t="e">
+        <f t="shared" si="20"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O31" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q31" s="2" t="e">
+        <f>_xlfn.CONFIDENCE.NORM(0.05, Q30, 10)</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="R31" s="2" t="e">
+        <f t="shared" ref="R31" si="21">_xlfn.CONFIDENCE.NORM(0.05, R30, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S31" s="2" t="e">
+        <f t="shared" ref="S31" si="22">_xlfn.CONFIDENCE.NORM(0.05, S30, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T31" s="2" t="e">
+        <f t="shared" ref="T31" si="23">_xlfn.CONFIDENCE.NORM(0.05, T30, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U31" s="2" t="e">
+        <f t="shared" ref="U31" si="24">_xlfn.CONFIDENCE.NORM(0.05, U30, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V31" s="2" t="e">
+        <f t="shared" ref="V31" si="25">_xlfn.CONFIDENCE.NORM(0.05, V30, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W31" s="2" t="e">
+        <f t="shared" ref="W31" si="26">_xlfn.CONFIDENCE.NORM(0.05, W30, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="X31" s="2" t="e">
+        <f t="shared" ref="X31" si="27">_xlfn.CONFIDENCE.NORM(0.05, X30, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Y31" s="2" t="e">
+        <f t="shared" ref="Y31" si="28">_xlfn.CONFIDENCE.NORM(0.05, Y30, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Z31" s="2" t="e">
+        <f t="shared" ref="Z31" si="29">_xlfn.CONFIDENCE.NORM(0.05, Z30, 10)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>